<commit_message>
Burndown und Präsi für Iteration 4
</commit_message>
<xml_diff>
--- a/Dokumentation/MS4/Burndown.xlsx
+++ b/Dokumentation/MS4/Burndown.xlsx
@@ -377,7 +377,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="23">
     <dxf>
       <font>
         <b/>
@@ -412,6 +412,42 @@
         <extend val="0"/>
         <color indexed="9"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -575,8 +611,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.38247699037620297"/>
-          <c:y val="1.9575856443719411E-2"/>
+          <c:x val="0.38247699037620342"/>
+          <c:y val="1.9575856443719425E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -594,8 +630,8 @@
           <c:yMode val="edge"/>
           <c:x val="6.3263041065482792E-2"/>
           <c:y val="0.11092985318107668"/>
-          <c:w val="0.78912319644839124"/>
-          <c:h val="0.79282218597063536"/>
+          <c:w val="0.78912319644839168"/>
+          <c:h val="0.79282218597063481"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -642,44 +678,41 @@
               <c:f>[0]!Desired_Trend</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.854166666666668</c:v>
+                  <c:v>20.68181818181818</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.958333333333332</c:v>
+                  <c:v>18.613636363636363</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.0625</c:v>
+                  <c:v>16.545454545454547</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.166666666666668</c:v>
+                  <c:v>14.477272727272727</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.270833333333334</c:v>
+                  <c:v>12.409090909090908</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.375</c:v>
+                  <c:v>10.340909090909092</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.4791666666666661</c:v>
+                  <c:v>8.2727272727272734</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.5833333333333339</c:v>
+                  <c:v>6.2045454545454533</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.6875</c:v>
+                  <c:v>4.1363636363636367</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.7916666666666679</c:v>
+                  <c:v>2.0681818181818166</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.8958333333333321</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -728,7 +761,7 @@
               <c:f>[0]!Actual_Days_Remaining</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>22.75</c:v>
                 </c:pt>
@@ -745,45 +778,36 @@
                   <c:v>17.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>16.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>13.45</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>12.45</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>8.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>8.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="79142912"/>
-        <c:axId val="79145600"/>
+        <c:axId val="41328640"/>
+        <c:axId val="41331328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79142912"/>
+        <c:axId val="41328640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -853,7 +877,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79145600"/>
+        <c:crossAx val="41331328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -862,7 +886,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79145600"/>
+        <c:axId val="41331328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -905,7 +929,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="1.2208724689406945E-2"/>
-              <c:y val="0.43230022178461169"/>
+              <c:y val="0.43230022178461208"/>
             </c:manualLayout>
           </c:layout>
           <c:spPr>
@@ -942,7 +966,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79142912"/>
+        <c:crossAx val="41328640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -962,9 +986,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86459489650160903"/>
-          <c:y val="0.47634588537670042"/>
-          <c:w val="0.13096554606043773"/>
+          <c:x val="0.86459489650160948"/>
+          <c:y val="0.47634588537670064"/>
+          <c:w val="0.13096554606043781"/>
           <c:h val="6.3621571147249978E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -1086,8 +1110,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="79739136"/>
-        <c:axId val="79745024"/>
+        <c:axId val="53459200"/>
+        <c:axId val="53465088"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1176,11 +1200,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="79739136"/>
-        <c:axId val="79745024"/>
+        <c:axId val="53459200"/>
+        <c:axId val="53465088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79739136"/>
+        <c:axId val="53459200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1204,14 +1228,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79745024"/>
+        <c:crossAx val="53465088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79745024"/>
+        <c:axId val="53465088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1236,7 +1260,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79739136"/>
+        <c:crossAx val="53459200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1247,10 +1271,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.77880952380952473"/>
+          <c:x val="0.77880952380952506"/>
           <c:y val="0.38324174513150894"/>
           <c:w val="0.20690476190476192"/>
-          <c:h val="0.20622139015839833"/>
+          <c:h val="0.20622139015839847"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -1293,7 +1317,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2237,55 +2261,55 @@
       <c r="B1" s="18"/>
       <c r="C1" s="14">
         <f>IF(ISNUMBER('Resource Allocation'!C$2),Sprint_Length-'Resource Allocation'!C$2+1,"")</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="14">
         <f>IF(ISNUMBER('Resource Allocation'!D$2),Sprint_Length-'Resource Allocation'!D$2+1,"")</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="14">
         <f>IF(ISNUMBER('Resource Allocation'!E$2),Sprint_Length-'Resource Allocation'!E$2+1,"")</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" s="14">
         <f>IF(ISNUMBER('Resource Allocation'!F$2),Sprint_Length-'Resource Allocation'!F$2+1,"")</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" s="14">
         <f>IF(ISNUMBER('Resource Allocation'!G$2),Sprint_Length-'Resource Allocation'!G$2+1,"")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H1" s="14">
         <f>IF(ISNUMBER('Resource Allocation'!H$2),Sprint_Length-'Resource Allocation'!H$2+1,"")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I1" s="14">
         <f>IF(ISNUMBER('Resource Allocation'!I$2),Sprint_Length-'Resource Allocation'!I$2+1,"")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J1" s="14">
         <f>IF(ISNUMBER('Resource Allocation'!J$2),Sprint_Length-'Resource Allocation'!J$2+1,"")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K1" s="14">
         <f>IF(ISNUMBER('Resource Allocation'!K$2),Sprint_Length-'Resource Allocation'!K$2+1,"")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L1" s="14">
         <f>IF(ISNUMBER('Resource Allocation'!L$2),Sprint_Length-'Resource Allocation'!L$2+1,"")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M1" s="14">
         <f>IF(ISNUMBER('Resource Allocation'!M$2),Sprint_Length-'Resource Allocation'!M$2+1,"")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N1" s="14">
         <f>IF(ISNUMBER('Resource Allocation'!N$2),Sprint_Length-'Resource Allocation'!N$2+1,"")</f>
-        <v>1</v>
-      </c>
-      <c r="O1" s="14">
+        <v>0</v>
+      </c>
+      <c r="O1" s="14" t="str">
         <f>IF(ISNUMBER('Resource Allocation'!O$2),Sprint_Length-'Resource Allocation'!O$2+1,"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="P1" s="14" t="str">
         <f>IF(ISNUMBER('Resource Allocation'!P$2),Sprint_Length-'Resource Allocation'!P$2+1,"")</f>
@@ -2703,9 +2727,9 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O2" s="7">
+      <c r="O2" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v/>
       </c>
       <c r="P2" s="7" t="str">
         <f t="shared" si="0"/>
@@ -3097,43 +3121,43 @@
       </c>
       <c r="H3" s="11">
         <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="I3" s="11">
+        <f ca="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="J3" s="11">
+        <f ca="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="K3" s="11">
+        <f ca="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="L3" s="11">
+        <f ca="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="M3" s="11">
+        <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="I3" s="11">
+      <c r="N3" s="11">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="J3" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="K3" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="L3" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="M3" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N3" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="O3" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="11">
-        <f ca="1"/>
-        <v>0</v>
+      <c r="O3" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="P3" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="Q3" s="11" t="str">
+        <f ca="1"/>
+        <v/>
       </c>
       <c r="R3" s="11" t="str">
         <f ca="1"/>
@@ -3517,43 +3541,43 @@
       </c>
       <c r="H4" s="11">
         <f ca="1"/>
+        <v>3.75</v>
+      </c>
+      <c r="I4" s="11">
+        <f ca="1"/>
+        <v>3.75</v>
+      </c>
+      <c r="J4" s="11">
+        <f ca="1"/>
+        <v>3.75</v>
+      </c>
+      <c r="K4" s="11">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="L4" s="11">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="M4" s="11">
+        <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="I4" s="11">
+      <c r="N4" s="11">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="J4" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="K4" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="M4" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N4" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="O4" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="P4" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="11">
-        <f ca="1"/>
-        <v>0</v>
+      <c r="O4" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="P4" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="Q4" s="11" t="str">
+        <f ca="1"/>
+        <v/>
       </c>
       <c r="R4" s="11" t="str">
         <f ca="1"/>
@@ -3937,43 +3961,43 @@
       </c>
       <c r="H5" s="11">
         <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="I5" s="11">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="J5" s="11">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="K5" s="11">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="L5" s="11">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M5" s="11">
+        <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="I5" s="11">
+      <c r="N5" s="11">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="J5" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="M5" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N5" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="P5" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="11">
-        <f ca="1"/>
-        <v>0</v>
+      <c r="O5" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="P5" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="Q5" s="11" t="str">
+        <f ca="1"/>
+        <v/>
       </c>
       <c r="R5" s="11" t="str">
         <f ca="1"/>
@@ -4337,11 +4361,11 @@
       </c>
       <c r="C6" s="11">
         <f t="array" ref="C6:DA6" ca="1">IF(Held_Standup,SUM(IF(Task_Owner=$B6,OFFSET('Burn Down'!$G$2,1,COLUMN()-3,Number_Tasks,1),0))/$A6,"")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="11">
         <f ca="1"/>
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="E6" s="11">
         <f ca="1"/>
@@ -4357,43 +4381,43 @@
       </c>
       <c r="H6" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="I6" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="J6" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="K6" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="L6" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="M6" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="N6" s="11">
         <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="11">
-        <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
+      </c>
+      <c r="O6" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="P6" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="Q6" s="11" t="str">
+        <f ca="1"/>
+        <v/>
       </c>
       <c r="R6" s="11" t="str">
         <f ca="1"/>
@@ -4757,12 +4781,12 @@
       </c>
       <c r="C7" s="11">
         <f t="array" ref="C7:DA7" ca="1">IF(Held_Standup,SUM(IF(Task_Owner=$B7,OFFSET('Burn Down'!$G$2,1,COLUMN()-3,Number_Tasks,1),0))/$A7,"")</f>
+        <v>2.75</v>
+      </c>
+      <c r="D7" s="11">
+        <f ca="1"/>
         <v>1.75</v>
       </c>
-      <c r="D7" s="11">
-        <f ca="1"/>
-        <v>1.25</v>
-      </c>
       <c r="E7" s="11">
         <f ca="1"/>
         <v>1</v>
@@ -4803,17 +4827,17 @@
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="O7" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="11">
-        <f ca="1"/>
-        <v>0</v>
+      <c r="O7" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="P7" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="Q7" s="11" t="str">
+        <f ca="1"/>
+        <v/>
       </c>
       <c r="R7" s="11" t="str">
         <f ca="1"/>
@@ -5196,43 +5220,43 @@
       </c>
       <c r="H8" s="12">
         <f ca="1">IF('Sprint Information'!G$52,SUM(OFFSET(H$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
+        <v>16.25</v>
       </c>
       <c r="I8" s="12">
         <f ca="1">IF('Sprint Information'!H$52,SUM(OFFSET(I$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
+        <v>13.45</v>
       </c>
       <c r="J8" s="12">
         <f ca="1">IF('Sprint Information'!I$52,SUM(OFFSET(J$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
+        <v>12.45</v>
       </c>
       <c r="K8" s="12">
         <f ca="1">IF('Sprint Information'!J$52,SUM(OFFSET(K$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="L8" s="12">
         <f ca="1">IF('Sprint Information'!K$52,SUM(OFFSET(L$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="M8" s="12">
         <f ca="1">IF('Sprint Information'!L$52,SUM(OFFSET(M$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="N8" s="12">
         <f ca="1">IF('Sprint Information'!M$52,SUM(OFFSET(N$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="O8" s="12" t="str">
         <f ca="1">IF('Sprint Information'!N$52,SUM(OFFSET(O$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="P8" s="12">
+        <v/>
+      </c>
+      <c r="P8" s="12" t="str">
         <f ca="1">IF('Sprint Information'!O$52,SUM(OFFSET(P$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="12">
+        <v/>
+      </c>
+      <c r="Q8" s="12" t="str">
         <f ca="1">IF('Sprint Information'!P$52,SUM(OFFSET(Q$2,1,0,ROW()-3,1)),"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="R8" s="12" t="str">
         <f ca="1">IF('Sprint Information'!Q$52,SUM(OFFSET(R$2,1,0,ROW()-3,1)),"")</f>
@@ -5590,20 +5614,20 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C9:DA65536 C3:DA7">
-    <cfRule type="cellIs" dxfId="19" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>C$1*Work_Hours_in_Day</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>C$1*Work_Hours_in_Day</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:IV8">
-    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="3" stopIfTrue="1">
       <formula>NOT(ISNUMBER(C$2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD2">
-    <cfRule type="cellIs" dxfId="16" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" stopIfTrue="1" operator="equal">
       <formula>Sprint_Length + 1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5622,7 +5646,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight" activeCell="R3" sqref="R3:R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelCol="1"/>
@@ -5658,55 +5682,55 @@
       </c>
       <c r="G1" s="14">
         <f>'Resource Allocation'!C1</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H1" s="14">
         <f>'Resource Allocation'!D1</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I1" s="14">
         <f>'Resource Allocation'!E1</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J1" s="14">
         <f>'Resource Allocation'!F1</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K1" s="14">
         <f>'Resource Allocation'!G1</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L1" s="14">
         <f>'Resource Allocation'!H1</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M1" s="14">
         <f>'Resource Allocation'!I1</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N1" s="14">
         <f>'Resource Allocation'!J1</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O1" s="14">
         <f>'Resource Allocation'!K1</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P1" s="14">
         <f>'Resource Allocation'!L1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q1" s="14">
         <f>'Resource Allocation'!M1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R1" s="14">
         <f>'Resource Allocation'!N1</f>
-        <v>1</v>
-      </c>
-      <c r="S1" s="14">
+        <v>0</v>
+      </c>
+      <c r="S1" s="14" t="str">
         <f>'Resource Allocation'!O1</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="T1" s="14" t="str">
         <f>'Resource Allocation'!P1</f>
@@ -6124,9 +6148,9 @@
         <f>'Resource Allocation'!N2</f>
         <v>12</v>
       </c>
-      <c r="S2" s="7">
+      <c r="S2" s="7" t="str">
         <f>'Resource Allocation'!O2</f>
-        <v>13</v>
+        <v/>
       </c>
       <c r="T2" s="7" t="str">
         <f>'Resource Allocation'!P2</f>
@@ -6514,13 +6538,27 @@
       <c r="K3" s="26">
         <v>0.5</v>
       </c>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
+      <c r="L3" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="M3" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="N3" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="O3" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="P3" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="Q3" s="27">
+        <v>0</v>
+      </c>
+      <c r="R3" s="27">
+        <v>0</v>
+      </c>
       <c r="S3" s="28"/>
       <c r="T3" s="28"/>
       <c r="U3" s="28"/>
@@ -6550,13 +6588,27 @@
       <c r="K4" s="26">
         <v>1</v>
       </c>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
+      <c r="L4" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="M4" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="N4" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="O4" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="P4" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="Q4" s="29">
+        <v>0</v>
+      </c>
+      <c r="R4" s="29">
+        <v>0</v>
+      </c>
       <c r="S4" s="30"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
@@ -6569,7 +6621,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G5" s="26">
         <v>1</v>
@@ -6607,15 +6659,9 @@
       <c r="R5" s="29">
         <v>0</v>
       </c>
-      <c r="S5" s="29">
-        <v>0</v>
-      </c>
-      <c r="T5" s="29">
-        <v>0</v>
-      </c>
-      <c r="U5" s="29">
-        <v>0</v>
-      </c>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
     </row>
     <row r="6" spans="1:109" ht="15">
       <c r="A6" s="4">
@@ -6642,14 +6688,28 @@
       <c r="K6" s="26">
         <v>5.25</v>
       </c>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
+      <c r="L6" s="26">
+        <v>5.25</v>
+      </c>
+      <c r="M6" s="26">
+        <v>5.25</v>
+      </c>
+      <c r="N6" s="26">
+        <v>5.25</v>
+      </c>
+      <c r="O6" s="26">
+        <v>5.25</v>
+      </c>
+      <c r="P6" s="26">
+        <v>5.25</v>
+      </c>
+      <c r="Q6" s="26">
+        <v>5.25</v>
+      </c>
+      <c r="R6" s="26">
+        <v>5.25</v>
+      </c>
+      <c r="S6" s="26"/>
       <c r="T6" s="29"/>
       <c r="U6" s="29"/>
     </row>
@@ -6678,13 +6738,27 @@
       <c r="K7" s="26">
         <v>2.5</v>
       </c>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
+      <c r="L7" s="26">
+        <v>2.5</v>
+      </c>
+      <c r="M7" s="26">
+        <v>2.5</v>
+      </c>
+      <c r="N7" s="26">
+        <v>1.5</v>
+      </c>
+      <c r="O7" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="P7" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="Q7" s="29">
+        <v>0</v>
+      </c>
+      <c r="R7" s="29">
+        <v>0</v>
+      </c>
       <c r="S7" s="29"/>
       <c r="T7" s="29"/>
       <c r="U7" s="29"/>
@@ -6714,13 +6788,27 @@
       <c r="K8" s="26">
         <v>2</v>
       </c>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
+      <c r="L8" s="26">
+        <v>2.5</v>
+      </c>
+      <c r="M8" s="26">
+        <v>1.5</v>
+      </c>
+      <c r="N8" s="26">
+        <v>1.5</v>
+      </c>
+      <c r="O8" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="P8" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="Q8" s="29">
+        <v>0</v>
+      </c>
+      <c r="R8" s="29">
+        <v>0</v>
+      </c>
       <c r="S8" s="29"/>
       <c r="T8" s="29"/>
       <c r="U8" s="29"/>
@@ -6750,13 +6838,27 @@
       <c r="K9" s="26">
         <v>1</v>
       </c>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
+      <c r="L9" s="26">
+        <v>1</v>
+      </c>
+      <c r="M9" s="26">
+        <v>0</v>
+      </c>
+      <c r="N9" s="26">
+        <v>0</v>
+      </c>
+      <c r="O9" s="26">
+        <v>0</v>
+      </c>
+      <c r="P9" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="26">
+        <v>0</v>
+      </c>
+      <c r="R9" s="26">
+        <v>0</v>
+      </c>
       <c r="S9" s="29"/>
       <c r="T9" s="29"/>
       <c r="U9" s="29"/>
@@ -6786,13 +6888,27 @@
       <c r="K10" s="26">
         <v>1</v>
       </c>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
+      <c r="L10" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="M10" s="26">
+        <v>0</v>
+      </c>
+      <c r="N10" s="26">
+        <v>0</v>
+      </c>
+      <c r="O10" s="26">
+        <v>0</v>
+      </c>
+      <c r="P10" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="26">
+        <v>0</v>
+      </c>
+      <c r="R10" s="26">
+        <v>0</v>
+      </c>
       <c r="S10" s="29"/>
       <c r="T10" s="29"/>
       <c r="U10" s="29"/>
@@ -6822,13 +6938,27 @@
       <c r="K11" s="26">
         <v>3.25</v>
       </c>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
+      <c r="L11" s="26">
+        <v>3.25</v>
+      </c>
+      <c r="M11" s="26">
+        <v>3.25</v>
+      </c>
+      <c r="N11" s="26">
+        <v>3.25</v>
+      </c>
+      <c r="O11" s="29">
+        <v>1.5</v>
+      </c>
+      <c r="P11" s="29">
+        <v>1.5</v>
+      </c>
+      <c r="Q11" s="29">
+        <v>0</v>
+      </c>
+      <c r="R11" s="29">
+        <v>0</v>
+      </c>
       <c r="S11" s="30"/>
       <c r="T11" s="30"/>
       <c r="U11" s="30"/>
@@ -6858,13 +6988,27 @@
       <c r="K12" s="26">
         <v>0.5</v>
       </c>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
+      <c r="L12" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="M12" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="N12" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="O12" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="P12" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="Q12" s="29">
+        <v>0</v>
+      </c>
+      <c r="R12" s="29">
+        <v>0</v>
+      </c>
       <c r="S12" s="29"/>
       <c r="T12" s="29"/>
       <c r="U12" s="29"/>
@@ -6915,15 +7059,9 @@
       <c r="R13" s="29">
         <v>0</v>
       </c>
-      <c r="S13" s="29">
-        <v>0</v>
-      </c>
-      <c r="T13" s="29">
-        <v>0</v>
-      </c>
-      <c r="U13" s="29">
-        <v>0</v>
-      </c>
+      <c r="S13" s="29"/>
+      <c r="T13" s="29"/>
+      <c r="U13" s="29"/>
     </row>
     <row r="14" spans="1:109" ht="15">
       <c r="A14" s="4">
@@ -6950,13 +7088,27 @@
       <c r="K14" s="26">
         <v>0.25</v>
       </c>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
+      <c r="L14" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="M14" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="N14" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="O14" s="29">
+        <v>0.25</v>
+      </c>
+      <c r="P14" s="29">
+        <v>0.25</v>
+      </c>
+      <c r="Q14" s="29">
+        <v>0.25</v>
+      </c>
+      <c r="R14" s="29">
+        <v>0.25</v>
+      </c>
       <c r="S14" s="29"/>
       <c r="T14" s="29"/>
       <c r="U14" s="29"/>
@@ -7134,56 +7286,71 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B24:B65536 B7:B21">
-    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="4" stopIfTrue="1">
       <formula>IF($F7=INDEX(Postponed_Values,1,1),TRUE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="5" stopIfTrue="1">
       <formula>IF(ISBLANK($G7),FALSE,OFFSET($G7,0,COUNT($G7:$DE7)-1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24:T65536 O22:T22 O3:P16 O19:P20 U3:DE65536 Q3:T20">
-    <cfRule type="expression" dxfId="13" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="G24:T65536 O22:T22 O19:P20 U3:DE65536 T3:T20 O3:S5 S7:S20 Q11:R20 O7:R8 O11:P16">
+    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
       <formula>AND($F3=INDEX(Postponed_Values,1,1),ISNUMBER(G$1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:B2 D2:IV2">
-    <cfRule type="cellIs" dxfId="12" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="7" stopIfTrue="1" operator="equal">
       <formula>Sprint_Length + 1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="8" stopIfTrue="1">
       <formula>AND(ISBLANK($C1),ISNUMBER($G1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="9" stopIfTrue="1">
       <formula>AND(VLOOKUP($C1,Commitment,3,FALSE)&gt;0,VLOOKUP($C1,Commitment,3,FALSE)&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="10" stopIfTrue="1">
       <formula>AND(VLOOKUP($C1,Commitment,3,FALSE)&lt;0,VLOOKUP($C1,Commitment,3,FALSE)&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
       <formula>IF($F4=INDEX(Postponed_Values,1,1),TRUE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="14" stopIfTrue="1">
       <formula>IF(ISBLANK($G4),FALSE,OFFSET($G4,0,COUNT($G4:$DE4)-1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="6" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="17" stopIfTrue="1">
       <formula>IF($F11=INDEX(Postponed_Values,1,1),TRUE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="18" stopIfTrue="1">
       <formula>IF(ISBLANK($G11),FALSE,OFFSET($G11,0,COUNT($G11:$DE11)-1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B6">
-    <cfRule type="expression" dxfId="4" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="21" stopIfTrue="1">
       <formula>IF($F22=INDEX(Postponed_Values,1,1),TRUE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="22" stopIfTrue="1">
       <formula>IF(ISBLANK($G22),FALSE,OFFSET($G22,0,COUNT($G22:$DE22)-1)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N12">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+      <formula>AND($F12=INDEX(Postponed_Values,1,1),ISNUMBER(N$1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M12">
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+      <formula>AND($F12=INDEX(Postponed_Values,1,1),ISNUMBER(M$1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L12">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+      <formula>AND($F12=INDEX(Postponed_Values,1,1),ISNUMBER(L$1))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -7785,55 +7952,55 @@
       </c>
       <c r="D1" s="14">
         <f>'Resource Allocation'!C$1</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="14">
         <f>'Resource Allocation'!D$1</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="14">
         <f>'Resource Allocation'!E$1</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G1" s="14">
         <f>'Resource Allocation'!F$1</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H1" s="14">
         <f>'Resource Allocation'!G$1</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I1" s="14">
         <f>'Resource Allocation'!H$1</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J1" s="14">
         <f>'Resource Allocation'!I$1</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K1" s="14">
         <f>'Resource Allocation'!J$1</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L1" s="14">
         <f>'Resource Allocation'!K$1</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M1" s="14">
         <f>'Resource Allocation'!L$1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N1" s="14">
         <f>'Resource Allocation'!M$1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O1" s="14">
         <f>'Resource Allocation'!N$1</f>
-        <v>1</v>
-      </c>
-      <c r="P1" s="14">
+        <v>0</v>
+      </c>
+      <c r="P1" s="14" t="str">
         <f>'Resource Allocation'!O$1</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="Q1" s="14" t="str">
         <f>'Resource Allocation'!P$1</f>
@@ -8256,9 +8423,9 @@
         <f>'Resource Allocation'!N$2</f>
         <v>12</v>
       </c>
-      <c r="P2" s="7">
+      <c r="P2" s="7" t="str">
         <f>'Resource Allocation'!O$2</f>
-        <v>13</v>
+        <v/>
       </c>
       <c r="Q2" s="7" t="str">
         <f>'Resource Allocation'!P$2</f>
@@ -8626,13 +8793,13 @@
         <f ca="1">IF(ROW()&gt;COUNTA(Resource)+3,"",OFFSET('Resource Allocation'!$B$1,ROW()-1,0))</f>
         <v>Andreas</v>
       </c>
-      <c r="B3" s="3" t="e">
+      <c r="B3" s="3">
         <f ca="1">IF(ROW()&gt;COUNTA(Resource)+2,"",IF(MATCH(FALSE,Held_Standup,-1)=1,"",OFFSET($D$1,0,MATCH(FALSE,Held_Standup,-1)-2)*OFFSET('Resource Allocation'!$A$2,ROW()-2,0)*Work_Hours_in_Day))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C3" s="16" t="str">
+        <v>0</v>
+      </c>
+      <c r="C3" s="16">
         <f t="shared" ref="C3:C32" ca="1" si="0">IF(ISNUMBER($B3),OFFSET($D3,0,MATCH(FALSE,Held_Standup,-1)-2)-$B3,"")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="D3" s="11">
         <f t="array" ref="D3:DB3" ca="1">IF(ROW()&gt;COUNTA(Resource)+3,"",IF(Held_Standup,IF(ROW()=COUNTA(Resource)+3,SUM(INDEX(OFFSET($D$2,1,0,ROW()-3,Sprint_Length+1),0,COLUMN()-3)),OFFSET('Resource Allocation'!$C$2,INDEX(ROW(),1,1)-2,0,1,103)*OFFSET('Resource Allocation'!$A$2,INDEX(ROW(),1,1)-2,0)),""))</f>
@@ -8656,43 +8823,43 @@
       </c>
       <c r="I3" s="11">
         <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="J3" s="11">
+        <f ca="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="K3" s="11">
+        <f ca="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="L3" s="11">
+        <f ca="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="M3" s="11">
+        <f ca="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="N3" s="11">
+        <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="J3" s="11">
+      <c r="O3" s="11">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="K3" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="L3" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="M3" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N3" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="O3" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="R3" s="11">
-        <f ca="1"/>
-        <v>0</v>
+      <c r="P3" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="Q3" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="R3" s="11" t="str">
+        <f ca="1"/>
+        <v/>
       </c>
       <c r="S3" s="11" t="str">
         <f ca="1"/>
@@ -9052,13 +9219,13 @@
         <f ca="1">IF(ROW()&gt;COUNTA(Resource)+3,"",OFFSET('Resource Allocation'!$B$1,ROW()-1,0))</f>
         <v>Mareike</v>
       </c>
-      <c r="B4" s="3" t="e">
+      <c r="B4" s="3">
         <f ca="1">IF(ROW()&gt;COUNTA(Resource)+2,"",IF(MATCH(FALSE,Held_Standup,-1)=1,"",OFFSET($D$1,0,MATCH(FALSE,Held_Standup,-1)-2)*OFFSET('Resource Allocation'!$A$2,ROW()-2,0)*Work_Hours_in_Day))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C4" s="16" t="str">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="D4" s="11">
         <f t="array" ref="D4:DB4" ca="1">IF(ROW()&gt;COUNTA(Resource)+3,"",IF(Held_Standup,IF(ROW()=COUNTA(Resource)+3,SUM(INDEX(OFFSET($D$2,1,0,ROW()-3,Sprint_Length+1),0,COLUMN()-3)),OFFSET('Resource Allocation'!$C$2,INDEX(ROW(),1,1)-2,0,1,103)*OFFSET('Resource Allocation'!$A$2,INDEX(ROW(),1,1)-2,0)),""))</f>
@@ -9082,43 +9249,43 @@
       </c>
       <c r="I4" s="11">
         <f ca="1"/>
+        <v>3.75</v>
+      </c>
+      <c r="J4" s="11">
+        <f ca="1"/>
+        <v>3.75</v>
+      </c>
+      <c r="K4" s="11">
+        <f ca="1"/>
+        <v>3.75</v>
+      </c>
+      <c r="L4" s="11">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="M4" s="11">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="N4" s="11">
+        <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="J4" s="11">
+      <c r="O4" s="11">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="K4" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="M4" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N4" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="O4" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="P4" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="R4" s="11">
-        <f ca="1"/>
-        <v>0</v>
+      <c r="P4" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="Q4" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="R4" s="11" t="str">
+        <f ca="1"/>
+        <v/>
       </c>
       <c r="S4" s="11" t="str">
         <f ca="1"/>
@@ -9478,13 +9645,13 @@
         <f ca="1">IF(ROW()&gt;COUNTA(Resource)+3,"",OFFSET('Resource Allocation'!$B$1,ROW()-1,0))</f>
         <v xml:space="preserve">Tom </v>
       </c>
-      <c r="B5" s="3" t="e">
+      <c r="B5" s="3">
         <f ca="1">IF(ROW()&gt;COUNTA(Resource)+2,"",IF(MATCH(FALSE,Held_Standup,-1)=1,"",OFFSET($D$1,0,MATCH(FALSE,Held_Standup,-1)-2)*OFFSET('Resource Allocation'!$A$2,ROW()-2,0)*Work_Hours_in_Day))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C5" s="16" t="str">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="D5" s="11">
         <f t="array" ref="D5:DB5" ca="1">IF(ROW()&gt;COUNTA(Resource)+3,"",IF(Held_Standup,IF(ROW()=COUNTA(Resource)+3,SUM(INDEX(OFFSET($D$2,1,0,ROW()-3,Sprint_Length+1),0,COLUMN()-3)),OFFSET('Resource Allocation'!$C$2,INDEX(ROW(),1,1)-2,0,1,103)*OFFSET('Resource Allocation'!$A$2,INDEX(ROW(),1,1)-2,0)),""))</f>
@@ -9508,43 +9675,43 @@
       </c>
       <c r="I5" s="11">
         <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="J5" s="11">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="K5" s="11">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="L5" s="11">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M5" s="11">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N5" s="11">
+        <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="J5" s="11">
+      <c r="O5" s="11">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="K5" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="M5" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="N5" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="P5" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="R5" s="11">
-        <f ca="1"/>
-        <v>0</v>
+      <c r="P5" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="Q5" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="R5" s="11" t="str">
+        <f ca="1"/>
+        <v/>
       </c>
       <c r="S5" s="11" t="str">
         <f ca="1"/>
@@ -9904,21 +10071,21 @@
         <f ca="1">IF(ROW()&gt;COUNTA(Resource)+3,"",OFFSET('Resource Allocation'!$B$1,ROW()-1,0))</f>
         <v>Tu</v>
       </c>
-      <c r="B6" s="3" t="e">
+      <c r="B6" s="3">
         <f ca="1">IF(ROW()&gt;COUNTA(Resource)+2,"",IF(MATCH(FALSE,Held_Standup,-1)=1,"",OFFSET($D$1,0,MATCH(FALSE,Held_Standup,-1)-2)*OFFSET('Resource Allocation'!$A$2,ROW()-2,0)*Work_Hours_in_Day))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C6" s="16" t="str">
+        <v>0</v>
+      </c>
+      <c r="C6" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>5.5</v>
       </c>
       <c r="D6" s="11">
         <f t="array" ref="D6:DB6" ca="1">IF(ROW()&gt;COUNTA(Resource)+3,"",IF(Held_Standup,IF(ROW()=COUNTA(Resource)+3,SUM(INDEX(OFFSET($D$2,1,0,ROW()-3,Sprint_Length+1),0,COLUMN()-3)),OFFSET('Resource Allocation'!$C$2,INDEX(ROW(),1,1)-2,0,1,103)*OFFSET('Resource Allocation'!$A$2,INDEX(ROW(),1,1)-2,0)),""))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="11">
         <f ca="1"/>
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="F6" s="11">
         <f ca="1"/>
@@ -9934,43 +10101,43 @@
       </c>
       <c r="I6" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="J6" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="K6" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="L6" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="M6" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="N6" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="O6" s="11">
         <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="R6" s="11">
-        <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
+      </c>
+      <c r="P6" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="Q6" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="R6" s="11" t="str">
+        <f ca="1"/>
+        <v/>
       </c>
       <c r="S6" s="11" t="str">
         <f ca="1"/>
@@ -10330,22 +10497,22 @@
         <f ca="1">IF(ROW()&gt;COUNTA(Resource)+3,"",OFFSET('Resource Allocation'!$B$1,ROW()-1,0))</f>
         <v>Sebastian</v>
       </c>
-      <c r="B7" s="3" t="e">
+      <c r="B7" s="3">
         <f ca="1">IF(ROW()&gt;COUNTA(Resource)+2,"",IF(MATCH(FALSE,Held_Standup,-1)=1,"",OFFSET($D$1,0,MATCH(FALSE,Held_Standup,-1)-2)*OFFSET('Resource Allocation'!$A$2,ROW()-2,0)*Work_Hours_in_Day))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C7" s="16" t="str">
+        <v>0</v>
+      </c>
+      <c r="C7" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="D7" s="11">
         <f t="array" ref="D7:DB7" ca="1">IF(ROW()&gt;COUNTA(Resource)+3,"",IF(Held_Standup,IF(ROW()=COUNTA(Resource)+3,SUM(INDEX(OFFSET($D$2,1,0,ROW()-3,Sprint_Length+1),0,COLUMN()-3)),OFFSET('Resource Allocation'!$C$2,INDEX(ROW(),1,1)-2,0,1,103)*OFFSET('Resource Allocation'!$A$2,INDEX(ROW(),1,1)-2,0)),""))</f>
+        <v>2.75</v>
+      </c>
+      <c r="E7" s="11">
+        <f ca="1"/>
         <v>1.75</v>
       </c>
-      <c r="E7" s="11">
-        <f ca="1"/>
-        <v>1.25</v>
-      </c>
       <c r="F7" s="11">
         <f ca="1"/>
         <v>1</v>
@@ -10386,17 +10553,17 @@
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="P7" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="11">
-        <f ca="1"/>
-        <v>0</v>
+      <c r="P7" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="Q7" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="R7" s="11" t="str">
+        <f ca="1"/>
+        <v/>
       </c>
       <c r="S7" s="11" t="str">
         <f ca="1"/>
@@ -10786,43 +10953,43 @@
       </c>
       <c r="I8" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>16.25</v>
       </c>
       <c r="J8" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>13.45</v>
       </c>
       <c r="K8" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>12.45</v>
       </c>
       <c r="L8" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="M8" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="N8" s="11">
         <f ca="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="O8" s="11">
         <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="11">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="11" t="e">
-        <f ca="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="R8" s="11" t="e">
-        <f ca="1"/>
-        <v>#REF!</v>
+        <v>5.5</v>
+      </c>
+      <c r="P8" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="Q8" s="11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="R8" s="11" t="str">
+        <f ca="1"/>
+        <v/>
       </c>
       <c r="S8" s="11" t="str">
         <f ca="1"/>
@@ -21852,7 +22019,7 @@
   <dimension ref="A1:FA60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -21867,7 +22034,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -21908,51 +22075,51 @@
       </c>
       <c r="C51" s="3">
         <f ca="1">IF(ISNUMBER('Resource Allocation'!D2),$B$51-('Resource Allocation'!C2*$B$51/'Sprint Information'!$B$1),"")</f>
-        <v>20.854166666666668</v>
+        <v>20.68181818181818</v>
       </c>
       <c r="D51" s="3">
         <f ca="1">IF(ISNUMBER('Resource Allocation'!E2),$B$51-('Resource Allocation'!D2*$B$51/'Sprint Information'!$B$1),"")</f>
-        <v>18.958333333333332</v>
+        <v>18.613636363636363</v>
       </c>
       <c r="E51" s="3">
         <f ca="1">IF(ISNUMBER('Resource Allocation'!F2),$B$51-('Resource Allocation'!E2*$B$51/'Sprint Information'!$B$1),"")</f>
-        <v>17.0625</v>
+        <v>16.545454545454547</v>
       </c>
       <c r="F51" s="3">
         <f ca="1">IF(ISNUMBER('Resource Allocation'!G2),$B$51-('Resource Allocation'!F2*$B$51/'Sprint Information'!$B$1),"")</f>
-        <v>15.166666666666668</v>
+        <v>14.477272727272727</v>
       </c>
       <c r="G51" s="3">
         <f ca="1">IF(ISNUMBER('Resource Allocation'!H2),$B$51-('Resource Allocation'!G2*$B$51/'Sprint Information'!$B$1),"")</f>
-        <v>13.270833333333334</v>
+        <v>12.409090909090908</v>
       </c>
       <c r="H51" s="3">
         <f ca="1">IF(ISNUMBER('Resource Allocation'!I2),$B$51-('Resource Allocation'!H2*$B$51/'Sprint Information'!$B$1),"")</f>
-        <v>11.375</v>
+        <v>10.340909090909092</v>
       </c>
       <c r="I51" s="3">
         <f ca="1">IF(ISNUMBER('Resource Allocation'!J2),$B$51-('Resource Allocation'!I2*$B$51/'Sprint Information'!$B$1),"")</f>
-        <v>9.4791666666666661</v>
+        <v>8.2727272727272734</v>
       </c>
       <c r="J51" s="3">
         <f ca="1">IF(ISNUMBER('Resource Allocation'!K2),$B$51-('Resource Allocation'!J2*$B$51/'Sprint Information'!$B$1),"")</f>
-        <v>7.5833333333333339</v>
+        <v>6.2045454545454533</v>
       </c>
       <c r="K51" s="3">
         <f ca="1">IF(ISNUMBER('Resource Allocation'!L2),$B$51-('Resource Allocation'!K2*$B$51/'Sprint Information'!$B$1),"")</f>
-        <v>5.6875</v>
+        <v>4.1363636363636367</v>
       </c>
       <c r="L51" s="3">
         <f ca="1">IF(ISNUMBER('Resource Allocation'!M2),$B$51-('Resource Allocation'!L2*$B$51/'Sprint Information'!$B$1),"")</f>
-        <v>3.7916666666666679</v>
+        <v>2.0681818181818166</v>
       </c>
       <c r="M51" s="3">
         <f ca="1">IF(ISNUMBER('Resource Allocation'!N2),$B$51-('Resource Allocation'!M2*$B$51/'Sprint Information'!$B$1),"")</f>
-        <v>1.8958333333333321</v>
-      </c>
-      <c r="N51" s="3">
-        <f ca="1">IF(ISNUMBER('Resource Allocation'!O2),$B$51-('Resource Allocation'!N2*$B$51/'Sprint Information'!$B$1),"")</f>
         <v>0</v>
+      </c>
+      <c r="N51" s="3" t="str">
+        <f>IF(ISNUMBER('Resource Allocation'!O2),$B$51-('Resource Allocation'!N2*$B$51/'Sprint Information'!$B$1),"")</f>
+        <v/>
       </c>
       <c r="O51" s="3" t="str">
         <f>IF(ISNUMBER('Resource Allocation'!P2),$B$51-('Resource Allocation'!O2*$B$51/'Sprint Information'!$B$1),"")</f>
@@ -22369,15 +22536,15 @@
       </c>
       <c r="N52" t="b">
         <f ca="1">COUNT(OFFSET('Burn Down'!$G$2,1,COLUMN()-2,Number_Tasks,1))&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O52" t="b">
         <f ca="1">COUNT(OFFSET('Burn Down'!$G$2,1,COLUMN()-2,Number_Tasks,1))&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P52" t="b">
         <f ca="1">COUNT(OFFSET('Burn Down'!$G$2,1,COLUMN()-2,Number_Tasks,1))&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q52" t="b">
         <f ca="1">COUNT(OFFSET('Burn Down'!$G$2,1,COLUMN()-2,Number_Tasks,1))&gt;0</f>
@@ -22795,9 +22962,9 @@
         <f>IF(ISNUMBER('Resource Allocation'!N$2),0,"")</f>
         <v>0</v>
       </c>
-      <c r="N54">
+      <c r="N54" t="str">
         <f>IF(ISNUMBER('Resource Allocation'!O$2),0,"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="O54" t="str">
         <f>IF(ISNUMBER('Resource Allocation'!P$2),0,"")</f>
@@ -24461,9 +24628,9 @@
       <c r="A60" t="s">
         <v>28</v>
       </c>
-      <c r="B60" t="e">
+      <c r="B60" t="str">
         <f ca="1">MID(CELL("filename"),FIND("[",CELL("filename"))+1,FIND("]",CELL("filename"))-FIND("[",CELL("filename"))-IF(MID(CELL("filename"),FIND("]",CELL("filename"))-4,1)=".",5,6))</f>
-        <v>#N/A</v>
+        <v>Burndown_ohneTu</v>
       </c>
     </row>
   </sheetData>

</xml_diff>